<commit_message>
referenties van alle result-files verwerkt
</commit_message>
<xml_diff>
--- a/method_selection/unusable_papers.xlsx
+++ b/method_selection/unusable_papers.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="9990" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="9990" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Different evaluation method" sheetId="1" r:id="rId1"/>
+    <sheet name="Different evaluation methodolog" sheetId="1" r:id="rId1"/>
     <sheet name="Different task" sheetId="2" r:id="rId2"/>
     <sheet name="Non-standard features" sheetId="3" r:id="rId3"/>
     <sheet name="No baseline performance" sheetId="4" r:id="rId4"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
   <si>
     <t>Methode</t>
   </si>
@@ -134,12 +134,6 @@
     <t>Transfer learning</t>
   </si>
   <si>
-    <t>RankAgg-NDCG</t>
-  </si>
-  <si>
-    <t>"Supervised ranking aggregation based on query similarity for document retrieval"</t>
-  </si>
-  <si>
     <t>"Semi-supervised Ranking via List-Wise Approach"</t>
   </si>
   <si>
@@ -365,9 +359,6 @@
     <t>QoRank</t>
   </si>
   <si>
-    <t>RankIP</t>
-  </si>
-  <si>
     <t>RankPSO</t>
   </si>
   <si>
@@ -377,10 +368,190 @@
     <t>RankSVM-Sigmoid</t>
   </si>
   <si>
-    <t>SSI</t>
-  </si>
-  <si>
     <t>XPGP</t>
+  </si>
+  <si>
+    <t>"Direct Optimization of Evaluation Measures ini Learning to Rank using Particle Swarm"</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>P@k</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>"Learning Structural SVMs with Latent Variables"</t>
+  </si>
+  <si>
+    <t>"Probabilistic Ranking Support Vector Machine"</t>
+  </si>
+  <si>
+    <t>"QoRank: A Query-Dependent Ranking Model Using LSE-Based Weighted Multiple Hyperplanes Aggregation for Information Retrieval"</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>"An efficient algorithm for learning to rank from preference graphs"</t>
+  </si>
+  <si>
+    <t>"Suppressing Outliers in Pairwise Preference Ranking"</t>
+  </si>
+  <si>
+    <t>"Learning Preferences with Hidden Common Cause Relations"</t>
+  </si>
+  <si>
+    <t>Monotone Retargeting</t>
+  </si>
+  <si>
+    <t>LETOR 4.0</t>
+  </si>
+  <si>
+    <t>"Learning to Rank With Bregman Divergences and Monotone Retargeting"</t>
+  </si>
+  <si>
+    <t>ListClonal</t>
+  </si>
+  <si>
+    <t>"Learning to Rank for Information Retrieval Using the Clonal Selection Algorithm"</t>
+  </si>
+  <si>
+    <t>MDDAG</t>
+  </si>
+  <si>
+    <t>"Fast classification using sparse decision DAGs"</t>
+  </si>
+  <si>
+    <t>LETOR 3.0, LETOR 4.0</t>
+  </si>
+  <si>
+    <t>RankMGP</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>"Applying Layered Multi-Population Genetic Programming on Learning to Rank for Information Retrieval"</t>
+  </si>
+  <si>
+    <t>Altered LETOR</t>
+  </si>
+  <si>
+    <t>BRE NW</t>
+  </si>
+  <si>
+    <t>CPS</t>
+  </si>
+  <si>
+    <t>CRF-agg</t>
+  </si>
+  <si>
+    <t>KTDispSq</t>
+  </si>
+  <si>
+    <t>RRA</t>
+  </si>
+  <si>
+    <t>SelectRanker</t>
+  </si>
+  <si>
+    <t>theta-MPM</t>
+  </si>
+  <si>
+    <t>"Ranking Aggregation Based on Belief Function Theory"</t>
+  </si>
+  <si>
+    <t>"A New Probabilistic Model for Rank Aggregation"</t>
+  </si>
+  <si>
+    <t>"CRF Framework for Supervised Preference Aggrgation"</t>
+  </si>
+  <si>
+    <t>"Displacement Based Unsupervised Metric for Evaluating Rank Aggregation"</t>
+  </si>
+  <si>
+    <t>"Rank Aggregation via Low-Rank and Structured-Sparse Decomposition"</t>
+  </si>
+  <si>
+    <t>"Query-Dependent Rank Aggregation with Local Models"</t>
+  </si>
+  <si>
+    <t>"A Flexible Generative Model for Preference Aggragation"</t>
+  </si>
+  <si>
+    <t>"An Extension of RankBoost for semi-supervised Learning of Ranking Functions"</t>
+  </si>
+  <si>
+    <t>AFS</t>
+  </si>
+  <si>
+    <t>ConeRank</t>
+  </si>
+  <si>
+    <t>"ConeRank: Ranking as Learning Generalized Inequalities"</t>
+  </si>
+  <si>
+    <t>VPRED</t>
+  </si>
+  <si>
+    <t>"Multi-stage Search Architectures for Streaming Documents"</t>
+  </si>
+  <si>
+    <t>RankBoost-Heter</t>
+  </si>
+  <si>
+    <t>RankBoost-semi</t>
+  </si>
+  <si>
+    <t>"Learning to Rank with Supplementary Data"</t>
+  </si>
+  <si>
+    <t>Risk-Sensitive Optimization</t>
+  </si>
+  <si>
+    <t>MSLR-web</t>
+  </si>
+  <si>
+    <t>"Robust Ranking Models via Risk-Sensitive Optimization"</t>
+  </si>
+  <si>
+    <t>iGBRT</t>
+  </si>
+  <si>
+    <t>RMSE, ERR, NDCg (mean)</t>
+  </si>
+  <si>
+    <t>"Web-Search Ranking with Initialized Gradient Boosted Regression Trees"</t>
+  </si>
+  <si>
+    <t>PreOrder</t>
+  </si>
+  <si>
+    <t>Yahoo!</t>
+  </si>
+  <si>
+    <t>"Learning Scoring Functions with Order-Preserving Losses and Standardized Supervision"</t>
+  </si>
+  <si>
+    <t>Cronus GBRT</t>
+  </si>
+  <si>
+    <t>Greedy Miser</t>
+  </si>
+  <si>
+    <t>Preference Perceptron</t>
+  </si>
+  <si>
+    <t>"Classifier Cascade for Minimizing Feature Evaluation Cost"</t>
+  </si>
+  <si>
+    <t>"The Greedy Miser: Learning under Test-time Budgets"</t>
+  </si>
+  <si>
+    <t>"Online Learning with Preference Feedback"</t>
   </si>
 </sst>
 </file>
@@ -427,9 +598,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,19 +879,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,10 +900,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -741,18 +914,24 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -762,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,21 +1104,21 @@
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -958,30 +1137,128 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
-        <v>97</v>
+      <c r="D22" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -991,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,13 +1289,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1029,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,13 +1341,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1069,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,299 +1404,387 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1396,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,68 +1818,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1491,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1956,7 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1511,52 +1964,80 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>116</v>
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
veel repetitief werk gedaan :(
</commit_message>
<xml_diff>
--- a/method_selection/unusable_papers.xlsx
+++ b/method_selection/unusable_papers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="9990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16695" windowHeight="9990" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Different evaluation methodolog" sheetId="1" r:id="rId1"/>
@@ -943,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1381,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -1946,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
raw data in appendix
</commit_message>
<xml_diff>
--- a/method_selection/unusable_papers.xlsx
+++ b/method_selection/unusable_papers.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="172">
   <si>
     <t>Methode</t>
   </si>
@@ -239,9 +239,6 @@
     <t>StructRank</t>
   </si>
   <si>
-    <t>VisGBT</t>
-  </si>
-  <si>
     <t>"Uncertainty-Based Active Ranking for Document Retrieval"</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
   </si>
   <si>
     <t>"Structured Ranking Learning using Cumulative Distribution Networks"</t>
-  </si>
-  <si>
-    <t>"VisGBT: Visually Analyzing Evolving Datasets for Adaptive Learning"</t>
   </si>
   <si>
     <t>ConvexLossNDCG</t>
@@ -882,7 +876,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -914,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -922,16 +916,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
         <v>132</v>
-      </c>
-      <c r="B3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -944,7 +938,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,119 +1140,119 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1271,7 +1265,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,13 +1294,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1314,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,24 +1346,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
         <v>159</v>
-      </c>
-      <c r="B3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1379,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,7 +1426,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,7 +1437,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1454,7 +1448,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1476,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1481,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,7 +1492,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1509,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1520,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,10 +1533,10 @@
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,7 +1580,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1608,7 +1602,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1619,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1630,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,7 +1635,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1657,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1685,40 +1679,40 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1726,7 +1720,7 @@
         <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
         <v>128</v>
@@ -1734,57 +1728,46 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
-      </c>
-      <c r="C32" t="s">
-        <v>130</v>
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>170</v>
-      </c>
-      <c r="B36" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1780,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,123 +1801,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
         <v>124</v>
-      </c>
-      <c r="B9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1947,7 +1930,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1972,72 +1955,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
         <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
         <v>116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" t="s">
         <v>162</v>
-      </c>
-      <c r="B6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>